<commit_message>
Added for update delete and get booking endpoints
</commit_message>
<xml_diff>
--- a/data/bookings.xlsx
+++ b/data/bookings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29" count="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28" count="33">
   <si>
     <t xml:space="preserve">firstname </t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">checkin </t>
   </si>
   <si>
-    <t xml:space="preserve">checkout </t>
+    <t>checkout</t>
   </si>
   <si>
     <t>additionalneeds</t>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">2018-01-01 </t>
   </si>
   <si>
-    <t xml:space="preserve">2019-01-01 </t>
-  </si>
-  <si>
     <t>Breakfast</t>
   </si>
   <si>
@@ -97,7 +94,7 @@
     <t>2019-14-01</t>
   </si>
   <si>
-    <t>2019-15-01</t>
+    <t>2019-14-02</t>
   </si>
   <si>
     <t>gfdd</t>
@@ -208,7 +205,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView topLeftCell="A1" view="normal" tabSelected="1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15"/>
@@ -258,102 +255,102 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
       </c>
       <c r="C3">
         <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
+      <c r="F3" s="1">
+        <v>43112</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
       <c r="C4">
         <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
+      <c r="F4" s="1">
+        <v>43110</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1">
-        <v>43113</v>
+        <v>43110</v>
       </c>
       <c r="F5" s="1">
-        <v>43469</v>
+        <v>43111</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
       <c r="C6">
         <v>20121</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>